<commit_message>
Sửa lỗi định dạng ngày tháng
</commit_message>
<xml_diff>
--- a/MaHH.xlsx
+++ b/MaHH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_hddt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CC44CC-AAA2-4DC0-9370-2FB190D617AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3863BF-8472-4B0E-81D7-D325B9CD2C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E1154C90-8187-4C9D-8DDB-7618463980C9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="323">
   <si>
     <t>Đvt</t>
   </si>
@@ -972,6 +972,36 @@
   </si>
   <si>
     <t>Mã hàng hóa</t>
+  </si>
+  <si>
+    <t>PV Engine RMI 15W-40/ 18 lít</t>
+  </si>
+  <si>
+    <t>PV Engine RMI 20W-50/ 18 lít</t>
+  </si>
+  <si>
+    <t>Vtech Ultra/ 4 lít</t>
+  </si>
+  <si>
+    <t>Vtech Super SAE 20W-50/ 4L</t>
+  </si>
+  <si>
+    <t>PV Engine HD 50/ 18 lít</t>
+  </si>
+  <si>
+    <t>Vspeed super 20W50 4T( lon 0,8 lít)</t>
+  </si>
+  <si>
+    <t>Dầu phanh DOT 3</t>
+  </si>
+  <si>
+    <t>VDMax Super 20W50/ 18L</t>
+  </si>
+  <si>
+    <t>VDMAax Plus 20W50/ 18L</t>
+  </si>
+  <si>
+    <t>PV Hydraulie VG 68M/ 18L</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1462,6 +1492,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1512,7 +1551,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1529,6 +1568,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="42" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1576,7 +1618,78 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1954,10 +2067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9639D367-352F-44BE-8505-63CC30B1FB0F}">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -3440,7 +3553,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
         <v>278</v>
       </c>
@@ -3451,7 +3564,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A136" s="2" t="s">
         <v>280</v>
       </c>
@@ -3462,7 +3575,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A137" s="2" t="s">
         <v>282</v>
       </c>
@@ -3473,7 +3586,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A138" s="2" t="s">
         <v>284</v>
       </c>
@@ -3484,7 +3597,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
         <v>286</v>
       </c>
@@ -3495,7 +3608,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
         <v>288</v>
       </c>
@@ -3506,7 +3619,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
         <v>290</v>
       </c>
@@ -3517,7 +3630,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
         <v>292</v>
       </c>
@@ -3528,7 +3641,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
         <v>294</v>
       </c>
@@ -3539,7 +3652,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
         <v>296</v>
       </c>
@@ -3550,7 +3663,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
         <v>298</v>
       </c>
@@ -3561,7 +3674,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
         <v>300</v>
       </c>
@@ -3572,7 +3685,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
         <v>302</v>
       </c>
@@ -3583,51 +3696,154 @@
         <v>301</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A148" s="3" t="s">
+    <row r="148" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A148" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D148" s="5"/>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A149" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A150" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A151" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A152" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A153" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A154" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A155" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A156" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A157" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B157" s="2"/>
+      <c r="C157" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A158" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A159" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A160" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A161" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C148" s="2" t="s">
+      <c r="B161" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A149" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A150" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A151" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C148 C150:C1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D148">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>